<commit_message>
read write file IO text
</commit_message>
<xml_diff>
--- a/Nề nếp.xlsx
+++ b/Nề nếp.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E51E88A-29B6-48BB-B57F-D267505E801B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4ACD5A7-76E7-4640-9972-91BBB37F7EDD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -115,6 +115,12 @@
     <t>31/3: đi trễ</t>
   </si>
   <si>
+    <t>Bảo</t>
+  </si>
+  <si>
+    <t>04/04; ko soạn bài</t>
+  </si>
+  <si>
     <t>10/03: Xin về sớm
 13/03: Đi trễ
 16/03: Đi trễ
@@ -122,13 +128,8 @@
 23/03: Chưa chuẩn bị bài
 29/03: Chưa làm bài
 30/03: Xin về sớm
-04/04: Ngủ quyên buổi chiều</t>
-  </si>
-  <si>
-    <t>Bảo</t>
-  </si>
-  <si>
-    <t>04/04; ko soạn bài</t>
+04/04: Ngủ quyên buổi
+07/04: đi trể chiều</t>
   </si>
 </sst>
 </file>
@@ -452,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,7 +491,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="123" customHeight="1" x14ac:dyDescent="0.25">
@@ -551,10 +552,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>